<commit_message>
Uni and multi here and categories (L1xL2) created and standardized with the rest Visuals for L1xL2 most frequent categories by type of analysis, next to each other
</commit_message>
<xml_diff>
--- a/othercatindicators.xlsx
+++ b/othercatindicators.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -535,7 +535,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>History of department transfers</t>
+          <t>Qualitative indices of antibiotic usage - Penicillins</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -544,17 +544,17 @@
         </is>
       </c>
       <c r="D5">
-        <v>9.34</v>
+        <v>5.25</v>
       </c>
       <c r="E5">
-        <v>5.13</v>
+        <v>1.45</v>
       </c>
       <c r="F5">
-        <v>16.99</v>
+        <v>19.03</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -564,19 +564,19 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>methicillin resistance</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>methicillin-resistant S. aureus</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Admission Diagnosis - Infections and allergic diseases</t>
+          <t>Antimicrobial and antifungal agents exposure within 3 mo -  aminoglycosides</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -585,17 +585,17 @@
         </is>
       </c>
       <c r="D6">
-        <v>4.24</v>
+        <v>3.02</v>
       </c>
       <c r="E6">
-        <v>2.45</v>
+        <v>1.01</v>
       </c>
       <c r="F6">
-        <v>7.34</v>
+        <v>9.06</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -610,14 +610,14 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>carbapenem-resistant P.aeruginosa</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Admission Diagnosis - Trauma</t>
+          <t>Antimicrobial and antifungal agents exposure within 3 mo - carbapenems</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -626,17 +626,17 @@
         </is>
       </c>
       <c r="D7">
-        <v>5.23</v>
+        <v>3.33</v>
       </c>
       <c r="E7">
-        <v>1.4</v>
+        <v>1.59</v>
       </c>
       <c r="F7">
-        <v>19.53</v>
+        <v>6.98</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -651,14 +651,14 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>carbapenem-resistant P.aeruginosa</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Pigtail use in previous 3 mo</t>
+          <t>Antibiotic Exposure - Cephalosporin</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -667,13 +667,13 @@
         </is>
       </c>
       <c r="D8">
-        <v>2.83</v>
+        <v>3.45</v>
       </c>
       <c r="E8">
-        <v>1.28</v>
+        <v>1.76</v>
       </c>
       <c r="F8">
-        <v>6.25</v>
+        <v>6.77</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -682,24 +682,24 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>resistance against multiple Watch antibiotics</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Antacid use</t>
+          <t>Antibiotic Exposure - Carbapenem</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -708,39 +708,39 @@
         </is>
       </c>
       <c r="D9">
-        <v>2.62</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="E9">
-        <v>1.38</v>
+        <v>4.8</v>
       </c>
       <c r="F9">
-        <v>4.99</v>
+        <v>16.38</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>vancomycin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>vancomycin-resistant Enterococci</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Carbapenems exposure</t>
+          <t>Antibiotic Exposure - Beta-lactam-beta-lactamase inhibitors</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -749,17 +749,17 @@
         </is>
       </c>
       <c r="D10">
-        <v>11.37</v>
+        <v>9.84</v>
       </c>
       <c r="E10">
-        <v>5.92</v>
+        <v>4.99</v>
       </c>
       <c r="F10">
-        <v>21.85</v>
+        <v>19.41</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -781,7 +781,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Î²-lactam/Î²-lactamase inhibitor combinations (BLBLIs) exposure</t>
+          <t>Antibiotic Exposure - Linezolid</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -790,17 +790,17 @@
         </is>
       </c>
       <c r="D11">
-        <v>10.41</v>
+        <v>8.24</v>
       </c>
       <c r="E11">
-        <v>5.65</v>
+        <v>2.71</v>
       </c>
       <c r="F11">
-        <v>19.19</v>
+        <v>25.08</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -822,7 +822,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Altered mental status</t>
+          <t>Antibiotic Exposure - Antifungals</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -831,17 +831,17 @@
         </is>
       </c>
       <c r="D12">
-        <v>10.56</v>
+        <v>6.14</v>
       </c>
       <c r="E12">
-        <v>5.27</v>
+        <v>2.38</v>
       </c>
       <c r="F12">
-        <v>21.17</v>
+        <v>15.87</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -863,7 +863,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Carbapenems exposure</t>
+          <t>Antibiotic Exposure - Vancomycin</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -872,17 +872,17 @@
         </is>
       </c>
       <c r="D13">
-        <v>6.21</v>
+        <v>6.18</v>
       </c>
       <c r="E13">
-        <v>3.1</v>
+        <v>1.28</v>
       </c>
       <c r="F13">
-        <v>12.44</v>
+        <v>29.77</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Î²-lactam/Î²-lactamase inhibitor combinations (BLBLIs) exposure</t>
+          <t>Pigtail use in previous 3 mo</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -913,39 +913,39 @@
         </is>
       </c>
       <c r="D14">
-        <v>5.66</v>
+        <v>2.83</v>
       </c>
       <c r="E14">
-        <v>2.91</v>
+        <v>1.28</v>
       </c>
       <c r="F14">
-        <v>10.99</v>
+        <v>6.25</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>resistance against multiple Watch antibiotics</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Altered mental status</t>
+          <t>Antacid use</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -954,13 +954,13 @@
         </is>
       </c>
       <c r="D15">
-        <v>5.69</v>
+        <v>2.62</v>
       </c>
       <c r="E15">
-        <v>2.75</v>
+        <v>1.38</v>
       </c>
       <c r="F15">
-        <v>11.79</v>
+        <v>4.99</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -969,24 +969,24 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>vancomycin resistance</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>vancomycin-resistant Enterococci</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Subjects with echocardiogram - both (transthoracic and transesophageal)</t>
+          <t>Any antibiotics exposure</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -995,13 +995,13 @@
         </is>
       </c>
       <c r="D16">
-        <v>17.16</v>
+        <v>15.06</v>
       </c>
       <c r="E16">
-        <v>1.96</v>
+        <v>8.119999999999999</v>
       </c>
       <c r="F16">
-        <v>150.23</v>
+        <v>27.92</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1015,19 +1015,19 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>vancomycin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>vancomycin-resistant Enterococci</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Chest X-ray finding - Pleural effusion</t>
+          <t>Carbapenems exposure</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1036,13 +1036,13 @@
         </is>
       </c>
       <c r="D17">
-        <v>3.8</v>
+        <v>11.37</v>
       </c>
       <c r="E17">
-        <v>1.48</v>
+        <v>5.92</v>
       </c>
       <c r="F17">
-        <v>9.76</v>
+        <v>21.85</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1056,19 +1056,19 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>methicillin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>methicillin-resistant S. aureus</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Transition to oral therapy</t>
+          <t>Î²-lactam/Î²-lactamase inhibitor combinations (BLBLIs) exposure</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1077,17 +1077,17 @@
         </is>
       </c>
       <c r="D18">
-        <v>0.1</v>
+        <v>10.41</v>
       </c>
       <c r="E18">
-        <v>0.05</v>
+        <v>5.65</v>
       </c>
       <c r="F18">
-        <v>0.21</v>
+        <v>19.19</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Adults &amp; pediatrics</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1109,7 +1109,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Comorbidities - Antifungal agents use within 30 days before BSI</t>
+          <t>Any antibiotics exposure</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1118,13 +1118,13 @@
         </is>
       </c>
       <c r="D19">
-        <v>5.07</v>
+        <v>10.75</v>
       </c>
       <c r="E19">
-        <v>2.67</v>
+        <v>4.78</v>
       </c>
       <c r="F19">
-        <v>9.630000000000001</v>
+        <v>24.19</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1150,7 +1150,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Underlying disease - None</t>
+          <t>Carbapenems exposure</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1159,17 +1159,17 @@
         </is>
       </c>
       <c r="D20">
-        <v>0.43</v>
+        <v>6.21</v>
       </c>
       <c r="E20">
-        <v>0.31</v>
+        <v>3.1</v>
       </c>
       <c r="F20">
-        <v>0.59</v>
+        <v>12.44</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1191,7 +1191,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Underlying disease - 1</t>
+          <t>Î²-lactam/Î²-lactamase inhibitor combinations (BLBLIs) exposure</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1200,17 +1200,17 @@
         </is>
       </c>
       <c r="D21">
-        <v>1.16</v>
+        <v>5.66</v>
       </c>
       <c r="E21">
-        <v>0.82</v>
+        <v>2.91</v>
       </c>
       <c r="F21">
-        <v>1.65</v>
+        <v>10.99</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1232,7 +1232,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Underlying disease - 2</t>
+          <t>Subjects with echocardiogram - both (transthoracic and transesophageal)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1241,17 +1241,17 @@
         </is>
       </c>
       <c r="D22">
-        <v>1.29</v>
+        <v>17.16</v>
       </c>
       <c r="E22">
-        <v>0.8100000000000001</v>
+        <v>1.96</v>
       </c>
       <c r="F22">
-        <v>2.06</v>
+        <v>150.23</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1261,19 +1261,19 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>vancomycin resistance</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>vancomycin-resistant Enterococci</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Underlying disease - 3</t>
+          <t>Chest X-ray finding - Pleural effusion</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1282,17 +1282,17 @@
         </is>
       </c>
       <c r="D23">
-        <v>1.8</v>
+        <v>3.8</v>
       </c>
       <c r="E23">
-        <v>0.92</v>
+        <v>1.48</v>
       </c>
       <c r="F23">
-        <v>3.53</v>
+        <v>9.76</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1302,19 +1302,19 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>methicillin resistance</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>methicillin-resistant S. aureus</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Underlying disease - â‰¥4</t>
+          <t>Transition to oral therapy</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1323,17 +1323,17 @@
         </is>
       </c>
       <c r="D24">
-        <v>3.25</v>
+        <v>0.1</v>
       </c>
       <c r="E24">
-        <v>1.98</v>
+        <v>0.05</v>
       </c>
       <c r="F24">
-        <v>5.35</v>
+        <v>0.21</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults &amp; pediatrics</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1355,7 +1355,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Oral stepdown</t>
+          <t>Comorbidities - Antifungal agents use within 30 days before BSI</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1364,13 +1364,13 @@
         </is>
       </c>
       <c r="D25">
-        <v>0.04</v>
+        <v>5.07</v>
       </c>
       <c r="E25">
-        <v>0.01</v>
+        <v>2.67</v>
       </c>
       <c r="F25">
-        <v>0.17</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1379,24 +1379,24 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Impaired mental status</t>
+          <t>Underlying disease - None</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1405,22 +1405,22 @@
         </is>
       </c>
       <c r="D26">
-        <v>64</v>
+        <v>0.43</v>
       </c>
       <c r="E26">
-        <v>9.199999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="F26">
-        <v>445.13</v>
+        <v>0.59</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1437,7 +1437,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>High-grade bacteremia (initial blood culture)</t>
+          <t>Oral stepdown</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1446,13 +1446,13 @@
         </is>
       </c>
       <c r="D27">
-        <v>0.39</v>
+        <v>0.04</v>
       </c>
       <c r="E27">
-        <v>0.16</v>
+        <v>0.01</v>
       </c>
       <c r="F27">
-        <v>0.9399999999999999</v>
+        <v>0.17</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1466,19 +1466,19 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>methicillin resistance</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>methicillin-resistant S. aureus</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>No. (%) of patients for whom a repeat blood culture was ordered</t>
+          <t>High-grade bacteremia (initial blood culture)</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1487,13 +1487,13 @@
         </is>
       </c>
       <c r="D28">
-        <v>6.73</v>
+        <v>0.39</v>
       </c>
       <c r="E28">
-        <v>1.48</v>
+        <v>0.16</v>
       </c>
       <c r="F28">
-        <v>30.51</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1507,19 +1507,19 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>MDR</t>
+          <t>methicillin resistance</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>methicillin-resistant S. aureus</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>No. (%) of patients for whom a repeat blood culture was ordered</t>
+          <t>Antibiotic exposures within 90 d - Antifungal prophylaxis</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1528,17 +1528,17 @@
         </is>
       </c>
       <c r="D29">
-        <v>19</v>
+        <v>2.58</v>
       </c>
       <c r="E29">
-        <v>6.31</v>
+        <v>1.28</v>
       </c>
       <c r="F29">
-        <v>57.23</v>
+        <v>5.18</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1548,19 +1548,19 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>MDR</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>carbapenem-resistant P.aeruginosa</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Background parameters - independent functional status (based on Katz criteria)</t>
+          <t>No. (%) of patients for whom a repeat blood culture was ordered</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1569,13 +1569,13 @@
         </is>
       </c>
       <c r="D30">
-        <v>0.15</v>
+        <v>6.73</v>
       </c>
       <c r="E30">
-        <v>0.1</v>
+        <v>1.48</v>
       </c>
       <c r="F30">
-        <v>0.23</v>
+        <v>30.51</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1589,19 +1589,19 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>MDR</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Any comorbidity</t>
+          <t>No. (%) of patients for whom a repeat blood culture was ordered</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1610,13 +1610,13 @@
         </is>
       </c>
       <c r="D31">
-        <v>5.39</v>
+        <v>19</v>
       </c>
       <c r="E31">
-        <v>1.22</v>
+        <v>6.31</v>
       </c>
       <c r="F31">
-        <v>23.85</v>
+        <v>57.23</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1630,19 +1630,19 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>MDR</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Predisposing factors (all)</t>
+          <t>Any comorbidity</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1651,13 +1651,13 @@
         </is>
       </c>
       <c r="D32">
-        <v>4.5</v>
+        <v>5.39</v>
       </c>
       <c r="E32">
-        <v>1.63</v>
+        <v>1.22</v>
       </c>
       <c r="F32">
-        <v>12.43</v>
+        <v>23.85</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1683,7 +1683,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Clinical infections - Yes</t>
+          <t>Predisposing factors (all)</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1692,39 +1692,39 @@
         </is>
       </c>
       <c r="D33">
-        <v>2.04</v>
+        <v>4.5</v>
       </c>
       <c r="E33">
-        <v>1.2</v>
+        <v>1.63</v>
       </c>
       <c r="F33">
-        <v>3.48</v>
+        <v>12.43</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Pediatrics</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>MDR but incorrectly or more extensively defined</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Fungi - Yes</t>
+          <t>Clinical infections - Yes</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1733,13 +1733,13 @@
         </is>
       </c>
       <c r="D34">
-        <v>8.75</v>
+        <v>2.04</v>
       </c>
       <c r="E34">
-        <v>3.63</v>
+        <v>1.2</v>
       </c>
       <c r="F34">
-        <v>21.08</v>
+        <v>3.48</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1765,7 +1765,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Trauma</t>
+          <t>Fungi - Yes</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1774,27 +1774,27 @@
         </is>
       </c>
       <c r="D35">
-        <v>0.22</v>
+        <v>8.75</v>
       </c>
       <c r="E35">
-        <v>0.06</v>
+        <v>3.63</v>
       </c>
       <c r="F35">
-        <v>0.8100000000000001</v>
+        <v>21.08</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>Pediatrics</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>fluoroquinolone resistance</t>
+          <t>MDR but incorrectly or more extensively defined</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -1806,7 +1806,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Fluoroquinolone use</t>
+          <t>Trauma</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1815,13 +1815,13 @@
         </is>
       </c>
       <c r="D36">
-        <v>6.17</v>
+        <v>0.22</v>
       </c>
       <c r="E36">
-        <v>2.76</v>
+        <v>0.06</v>
       </c>
       <c r="F36">
-        <v>13.77</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -1847,7 +1847,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Urgent hospital admission</t>
+          <t>Fluoroquinolone use</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1856,17 +1856,17 @@
         </is>
       </c>
       <c r="D37">
-        <v>0.23</v>
+        <v>6.17</v>
       </c>
       <c r="E37">
-        <v>0.1</v>
+        <v>2.76</v>
       </c>
       <c r="F37">
-        <v>0.55</v>
+        <v>13.77</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1876,19 +1876,19 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>fluoroquinolone resistance</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Overall survival at 1 year after onset of BSI - in adults</t>
+          <t>Urgent hospital admission</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1897,39 +1897,39 @@
         </is>
       </c>
       <c r="D38">
-        <v>0.63</v>
+        <v>0.23</v>
       </c>
       <c r="E38">
-        <v>0.22</v>
+        <v>0.1</v>
       </c>
       <c r="F38">
-        <v>1.77</v>
+        <v>0.55</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Adults &amp; pediatrics</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>vancomycin resistance</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>vancomycin-resistant Enterococci</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Fluoroquinolones</t>
+          <t>Exposure to antibiotics-Exposure to any antibiotics</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1938,13 +1938,13 @@
         </is>
       </c>
       <c r="D39">
-        <v>2.4</v>
+        <v>21.54</v>
       </c>
       <c r="E39">
-        <v>1.31</v>
+        <v>6.61</v>
       </c>
       <c r="F39">
-        <v>4.39</v>
+        <v>70.15000000000001</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1953,24 +1953,24 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Carbapenems</t>
+          <t>Exposure to antibiotics-Penicillin</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1979,13 +1979,13 @@
         </is>
       </c>
       <c r="D40">
-        <v>2.58</v>
+        <v>4.29</v>
       </c>
       <c r="E40">
-        <v>1.21</v>
+        <v>2.59</v>
       </c>
       <c r="F40">
-        <v>5.52</v>
+        <v>7.1</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1994,24 +1994,24 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Predisposing factors - Any predisposing condition</t>
+          <t>Exposure to antibiotics-Carbapenems</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2020,17 +2020,17 @@
         </is>
       </c>
       <c r="D41">
-        <v>1.69</v>
+        <v>4.96</v>
       </c>
       <c r="E41">
-        <v>0.97</v>
+        <v>2.89</v>
       </c>
       <c r="F41">
-        <v>2.93</v>
+        <v>8.51</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Adults &amp; pediatrics</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2040,19 +2040,19 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>methicillin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>methicillin-resistant S. aureus</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Thrombosis</t>
+          <t>Exposure to antibiotics-Quinolones</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2061,17 +2061,17 @@
         </is>
       </c>
       <c r="D42">
-        <v>3.52</v>
+        <v>3.5</v>
       </c>
       <c r="E42">
-        <v>1.4</v>
+        <v>2.04</v>
       </c>
       <c r="F42">
-        <v>8.859999999999999</v>
+        <v>6</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pediatrics</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2081,19 +2081,19 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>methicillin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>methicillin-resistant S. aureus</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Infectious disease as an admission diagnosis</t>
+          <t>Exposure to antibiotics-Vancomycin</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2102,13 +2102,13 @@
         </is>
       </c>
       <c r="D43">
-        <v>2.68</v>
+        <v>3.48</v>
       </c>
       <c r="E43">
-        <v>1.4</v>
+        <v>2.11</v>
       </c>
       <c r="F43">
-        <v>5.13</v>
+        <v>5.74</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -2122,19 +2122,19 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>MDR but incorrectly or more extensively defined</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Prolonged use of multiple antibiotics for 7 days-No</t>
+          <t>Exposure to antibiotics-Macrolides</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2143,17 +2143,17 @@
         </is>
       </c>
       <c r="D44">
-        <v>0.02</v>
+        <v>8.5</v>
       </c>
       <c r="E44">
-        <v>0.01</v>
+        <v>3.51</v>
       </c>
       <c r="F44">
-        <v>0.06</v>
+        <v>20.59</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2163,19 +2163,19 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>vancomycin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>vancomycin-resistant Enterococci</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Exposure to devices-No exposure</t>
+          <t>Exposure to antibiotics-Aminoglycosides</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2184,17 +2184,17 @@
         </is>
       </c>
       <c r="D45">
-        <v>0.47</v>
+        <v>2.98</v>
       </c>
       <c r="E45">
-        <v>0.18</v>
+        <v>1.47</v>
       </c>
       <c r="F45">
-        <v>1.24</v>
+        <v>6.03</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2204,19 +2204,19 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>vancomycin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>vancomycin-resistant Enterococci</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Vancomycin</t>
+          <t>Exposure to antibiotics-Colistin</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2225,39 +2225,39 @@
         </is>
       </c>
       <c r="D46">
-        <v>6.33</v>
+        <v>12.02</v>
       </c>
       <c r="E46">
-        <v>1.97</v>
+        <v>4.42</v>
       </c>
       <c r="F46">
-        <v>20.31</v>
+        <v>32.7</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>vancomycin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>vancomycin-resistant Enterococci</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>No. of prior courses of BL/FQ - Within 90 days of bloodstream - infection - 0</t>
+          <t>Fluoroquinolones</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2266,13 +2266,13 @@
         </is>
       </c>
       <c r="D47">
-        <v>0.11</v>
+        <v>2.4</v>
       </c>
       <c r="E47">
-        <v>0.06</v>
+        <v>1.31</v>
       </c>
       <c r="F47">
-        <v>0.21</v>
+        <v>4.39</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2281,7 +2281,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -2298,7 +2298,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Oral Antibiotics at Discharge</t>
+          <t>Carbapenems</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2307,39 +2307,39 @@
         </is>
       </c>
       <c r="D48">
-        <v>0.28</v>
+        <v>2.58</v>
       </c>
       <c r="E48">
-        <v>0.09</v>
+        <v>1.21</v>
       </c>
       <c r="F48">
-        <v>0.9</v>
+        <v>5.52</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Pediatrics</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>methicillin resistance</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>methicillin-resistant S. aureus</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Therapeutic management - Infectious disease consultation</t>
+          <t>Previous antibiotic exposure (within 1 month) - Antifungal drugs</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2348,39 +2348,39 @@
         </is>
       </c>
       <c r="D49">
-        <v>0.57</v>
+        <v>3.29</v>
       </c>
       <c r="E49">
-        <v>0.37</v>
+        <v>1.01</v>
       </c>
       <c r="F49">
-        <v>0.89</v>
+        <v>10.69</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>Neonates</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>methicillin resistance</t>
+          <t>multiple AMR profiles combined</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>methicillin-resistant S. aureus</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Transthoracic echocardiography performed</t>
+          <t>Predisposing factors - Any predisposing condition</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2389,17 +2389,17 @@
         </is>
       </c>
       <c r="D50">
-        <v>0.71</v>
+        <v>1.69</v>
       </c>
       <c r="E50">
-        <v>0.55</v>
+        <v>0.97</v>
       </c>
       <c r="F50">
-        <v>0.92</v>
+        <v>2.93</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>Adults &amp; pediatrics</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2421,7 +2421,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Management of S. aureus-BSI - trans-thoracic echocardiography performed</t>
+          <t>Thrombosis</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2430,17 +2430,17 @@
         </is>
       </c>
       <c r="D51">
-        <v>0.71</v>
+        <v>3.52</v>
       </c>
       <c r="E51">
-        <v>0.55</v>
+        <v>1.4</v>
       </c>
       <c r="F51">
-        <v>0.92</v>
+        <v>8.859999999999999</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>Pediatrics</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2462,7 +2462,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Underlying disease</t>
+          <t>Infectious disease as an admission diagnosis</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2471,17 +2471,17 @@
         </is>
       </c>
       <c r="D52">
-        <v>4.31</v>
+        <v>2.68</v>
       </c>
       <c r="E52">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="F52">
-        <v>15.51</v>
+        <v>5.13</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Pediatrics incl. neonates</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2491,19 +2491,19 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>MDR but incorrectly or more extensively defined</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Change in antibiotic treatment after the positive culture</t>
+          <t>Prolonged use of multiple antibiotics for 7 days-No</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2512,17 +2512,17 @@
         </is>
       </c>
       <c r="D53">
-        <v>2.04</v>
+        <v>0.02</v>
       </c>
       <c r="E53">
-        <v>1.02</v>
+        <v>0.01</v>
       </c>
       <c r="F53">
-        <v>4.1</v>
+        <v>0.06</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Pediatrics incl. neonates</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -2532,19 +2532,19 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>vancomycin resistance</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>vancomycin-resistant Enterococci</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Suspected diagnosis at admission - SSTI</t>
+          <t>Exposure to devices-No exposure</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2553,17 +2553,17 @@
         </is>
       </c>
       <c r="D54">
-        <v>0.13</v>
+        <v>0.47</v>
       </c>
       <c r="E54">
-        <v>0.03</v>
+        <v>0.18</v>
       </c>
       <c r="F54">
-        <v>0.5600000000000001</v>
+        <v>1.24</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -2573,19 +2573,19 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>vancomycin resistance</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>vancomycin-resistant Enterococci</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Source control intervention performed</t>
+          <t>Intrinsic and extrinsic risk factors associated with a BSI due to E. coli producing ampC-type enzymes - At least one risk factor</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2594,17 +2594,17 @@
         </is>
       </c>
       <c r="D55">
-        <v>2.49</v>
+        <v>22.86</v>
       </c>
       <c r="E55">
-        <v>1.6</v>
+        <v>2.44</v>
       </c>
       <c r="F55">
-        <v>3.88</v>
+        <v>214.59</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Pediatrics incl. neonates</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -2614,19 +2614,19 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>methicillin resistance</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>methicillin-resistant S. aureus</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Antibiotic Tx before KP isolation - antifungals</t>
+          <t>Vancomycin</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2635,39 +2635,39 @@
         </is>
       </c>
       <c r="D56">
-        <v>8.57</v>
+        <v>6.33</v>
       </c>
       <c r="E56">
-        <v>4.24</v>
+        <v>1.97</v>
       </c>
       <c r="F56">
-        <v>17.32</v>
+        <v>20.31</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>vancomycin resistance</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>vancomycin-resistant Enterococci</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Source of bloodstream infection - endogenous source</t>
+          <t>No. of prior courses of BL/FQ - Within 90 days of bloodstream - infection - 0</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2676,13 +2676,13 @@
         </is>
       </c>
       <c r="D57">
-        <v>0.8100000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="E57">
-        <v>0.62</v>
+        <v>0.06</v>
       </c>
       <c r="F57">
-        <v>1.06</v>
+        <v>0.21</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2691,24 +2691,24 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>MDR</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Grade III-IV mucositis</t>
+          <t>Oral Antibiotics at Discharge</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2717,39 +2717,39 @@
         </is>
       </c>
       <c r="D58">
-        <v>1.66</v>
+        <v>0.28</v>
       </c>
       <c r="E58">
-        <v>1.17</v>
+        <v>0.09</v>
       </c>
       <c r="F58">
-        <v>2.35</v>
+        <v>0.9</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>Pediatrics</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>MDR</t>
+          <t>methicillin resistance</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>methicillin-resistant S. aureus</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>History of valve disease on native valve - Congenital valve disease</t>
+          <t>Therapeutic management - Infectious disease consultation</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2758,10 +2758,13 @@
         </is>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>0.57</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>0.37</v>
+      </c>
+      <c r="F59">
+        <v>0.89</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2787,7 +2790,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Echocardiographic findings during IE - Perivalvular lesion</t>
+          <t>Transthoracic echocardiography performed</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2796,13 +2799,13 @@
         </is>
       </c>
       <c r="D60">
-        <v>0.46</v>
+        <v>0.71</v>
       </c>
       <c r="E60">
-        <v>0.22</v>
+        <v>0.55</v>
       </c>
       <c r="F60">
-        <v>0.97</v>
+        <v>0.92</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2828,7 +2831,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Type of admission - Traumatic</t>
+          <t>Management of S. aureus-BSI - trans-thoracic echocardiography performed</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2837,13 +2840,13 @@
         </is>
       </c>
       <c r="D61">
-        <v>0.21</v>
+        <v>0.71</v>
       </c>
       <c r="E61">
-        <v>0.07000000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="F61">
-        <v>0.62</v>
+        <v>0.92</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2852,24 +2855,24 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>methicillin resistance</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>methicillin-resistant S. aureus</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Active infection at admission</t>
+          <t>Management of S. aureus-BSI - regimen modified based on susceptibility test results</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2878,13 +2881,13 @@
         </is>
       </c>
       <c r="D62">
-        <v>2.72</v>
+        <v>0.35</v>
       </c>
       <c r="E62">
-        <v>1.28</v>
+        <v>0.26</v>
       </c>
       <c r="F62">
-        <v>5.79</v>
+        <v>0.46</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2893,24 +2896,24 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>methicillin resistance</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>methicillin-resistant S. aureus</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Maternal risk factors - Firstborn</t>
+          <t>Empiric therapy - Others</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2919,39 +2922,36 @@
         </is>
       </c>
       <c r="D63">
-        <v>4.78</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>1.36</v>
-      </c>
-      <c r="F63">
-        <v>16.79</v>
+        <v>0</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Neonates</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>MDR</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Maternal risk factors - in vitro fertilization</t>
+          <t>Underlying disease</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2960,39 +2960,39 @@
         </is>
       </c>
       <c r="D64">
-        <v>8.94</v>
+        <v>4.31</v>
       </c>
       <c r="E64">
-        <v>2.06</v>
+        <v>1.2</v>
       </c>
       <c r="F64">
-        <v>38.84</v>
+        <v>15.51</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Neonates</t>
+          <t>Pediatrics incl. neonates</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>MDR</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Severe  intraventricular haemorrhage (IVH)</t>
+          <t>Change in antibiotic treatment after the positive culture</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -3001,39 +3001,39 @@
         </is>
       </c>
       <c r="D65">
-        <v>22.15</v>
+        <v>2.04</v>
       </c>
       <c r="E65">
-        <v>6.47</v>
+        <v>1.02</v>
       </c>
       <c r="F65">
-        <v>75.84</v>
+        <v>4.1</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Neonates</t>
+          <t>Pediatrics incl. neonates</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>MDR</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Inotropes</t>
+          <t>Previous antifungal agents (&lt;90 days)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -3042,39 +3042,39 @@
         </is>
       </c>
       <c r="D66">
-        <v>10.62</v>
+        <v>3.03</v>
       </c>
       <c r="E66">
-        <v>3.68</v>
+        <v>1.47</v>
       </c>
       <c r="F66">
-        <v>30.62</v>
+        <v>6.24</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Neonates</t>
+          <t>Pediatrics incl. neonates</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>MDR</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Antibiotics-Cephalosporins</t>
+          <t>Source control intervention performed</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -3083,39 +3083,39 @@
         </is>
       </c>
       <c r="D67">
-        <v>0.41</v>
+        <v>2.49</v>
       </c>
       <c r="E67">
-        <v>0.26</v>
+        <v>1.6</v>
       </c>
       <c r="F67">
-        <v>0.65</v>
+        <v>3.88</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>Pediatrics incl. neonates</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>methicillin resistance</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>methicillin-resistant S. aureus</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Antibiotics-Cefazolin</t>
+          <t>Antibiotic exposure - Antifungal agent</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -3124,13 +3124,13 @@
         </is>
       </c>
       <c r="D68">
-        <v>0.03</v>
+        <v>3.74</v>
       </c>
       <c r="E68">
-        <v>0.01</v>
+        <v>2.16</v>
       </c>
       <c r="F68">
-        <v>0.08</v>
+        <v>6.48</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -3139,24 +3139,24 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>carbapenem-resistant P.aeruginosa</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Antibiotics-Ceftazidime</t>
+          <t>Antibiotic Tx before KP isolation - antifungals</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -3165,13 +3165,13 @@
         </is>
       </c>
       <c r="D69">
-        <v>0.32</v>
+        <v>8.57</v>
       </c>
       <c r="E69">
-        <v>0.22</v>
+        <v>4.24</v>
       </c>
       <c r="F69">
-        <v>0.47</v>
+        <v>17.32</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -3180,24 +3180,24 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>carbapenem resistance</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>carbapenem-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Antibiotics-Cefepime</t>
+          <t>Grade III-IV mucositis</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -3206,13 +3206,13 @@
         </is>
       </c>
       <c r="D70">
-        <v>0.37</v>
+        <v>1.66</v>
       </c>
       <c r="E70">
-        <v>0.25</v>
+        <v>1.17</v>
       </c>
       <c r="F70">
-        <v>0.55</v>
+        <v>2.35</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -3226,19 +3226,19 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>MDR</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>B-lactam/B-lactamase inhibitor-Piperacillin-tazobactam</t>
+          <t>History of valve disease on native valve - Congenital valve disease</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -3247,13 +3247,10 @@
         </is>
       </c>
       <c r="D71">
-        <v>3.09</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>1.85</v>
-      </c>
-      <c r="F71">
-        <v>5.17</v>
+        <v>0</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -3262,24 +3259,24 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>methicillin resistance</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>methicillin-resistant S. aureus</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Aztreonam</t>
+          <t>Echocardiographic findings during IE - Perivalvular lesion</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3288,13 +3285,13 @@
         </is>
       </c>
       <c r="D72">
-        <v>0.28</v>
+        <v>0.46</v>
       </c>
       <c r="E72">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="F72">
-        <v>0.41</v>
+        <v>0.97</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -3303,24 +3300,24 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>methicillin resistance</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>methicillin-resistant S. aureus</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Aminoglycosides-Gentamicin</t>
+          <t>Maternal risk factors - Firstborn</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3329,17 +3326,17 @@
         </is>
       </c>
       <c r="D73">
-        <v>0.48</v>
+        <v>4.78</v>
       </c>
       <c r="E73">
-        <v>0.33</v>
+        <v>1.36</v>
       </c>
       <c r="F73">
-        <v>0.7</v>
+        <v>16.79</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>Neonates</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -3349,19 +3346,19 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>MDR</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Aminoglycosides-Tobramycin</t>
+          <t>Maternal risk factors - in vitro fertilization</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -3370,17 +3367,17 @@
         </is>
       </c>
       <c r="D74">
-        <v>0.48</v>
+        <v>8.94</v>
       </c>
       <c r="E74">
-        <v>0.32</v>
+        <v>2.06</v>
       </c>
       <c r="F74">
-        <v>0.73</v>
+        <v>38.84</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>Neonates</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -3390,19 +3387,19 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>MDR</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Sulfonamides-Sulfame-thoxazole</t>
+          <t>Severe  intraventricular haemorrhage (IVH)</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -3411,17 +3408,17 @@
         </is>
       </c>
       <c r="D75">
-        <v>0.52</v>
+        <v>22.15</v>
       </c>
       <c r="E75">
-        <v>0.35</v>
+        <v>6.47</v>
       </c>
       <c r="F75">
-        <v>0.77</v>
+        <v>75.84</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>Neonates</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -3431,19 +3428,19 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>3rd gen cephalosporin resistance</t>
+          <t>MDR</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>C3G-resistant Enterobacterales</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Ultimately or rapidly fatal underlying disease</t>
+          <t>Inotropes</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -3452,27 +3449,27 @@
         </is>
       </c>
       <c r="D76">
-        <v>2.08</v>
+        <v>10.62</v>
       </c>
       <c r="E76">
-        <v>1.64</v>
+        <v>3.68</v>
       </c>
       <c r="F76">
-        <v>2.64</v>
+        <v>30.62</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Neonates</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>resistance against multiple Watch antibiotics</t>
+          <t>MDR</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
@@ -3484,7 +3481,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Prior antifungal exposure</t>
+          <t>Antibiotics-Cephalosporins</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3493,39 +3490,39 @@
         </is>
       </c>
       <c r="D77">
-        <v>3.92</v>
+        <v>0.41</v>
       </c>
       <c r="E77">
-        <v>1.35</v>
+        <v>0.26</v>
       </c>
       <c r="F77">
-        <v>11.37</v>
+        <v>0.65</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>All ages or not specified</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>resistance against multiple Watch antibiotics</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Time between admission and index culture days - 1 day prior to admission</t>
+          <t>Antibiotics-Cefazolin</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3534,13 +3531,13 @@
         </is>
       </c>
       <c r="D78">
-        <v>1.05</v>
+        <v>0.03</v>
       </c>
       <c r="E78">
-        <v>0.68</v>
+        <v>0.01</v>
       </c>
       <c r="F78">
-        <v>1.63</v>
+        <v>0.08</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -3549,24 +3546,24 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Time between admission and index culture days - Same day as admission</t>
+          <t>Antibiotics-Ceftazidime</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -3575,13 +3572,13 @@
         </is>
       </c>
       <c r="D79">
-        <v>0.48</v>
+        <v>0.32</v>
       </c>
       <c r="E79">
-        <v>0.35</v>
+        <v>0.22</v>
       </c>
       <c r="F79">
-        <v>0.65</v>
+        <v>0.47</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -3590,24 +3587,24 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Type of infection - Bacteraemia</t>
+          <t>Antibiotics-Cefepime</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -3616,13 +3613,13 @@
         </is>
       </c>
       <c r="D80">
-        <v>4.68</v>
+        <v>0.37</v>
       </c>
       <c r="E80">
-        <v>1.79</v>
+        <v>0.25</v>
       </c>
       <c r="F80">
-        <v>12.23</v>
+        <v>0.55</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -3631,24 +3628,24 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>MDR</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Receipt of inotropic drug</t>
+          <t>B-lactam/B-lactamase inhibitor-Piperacillin-tazobactam</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -3657,13 +3654,13 @@
         </is>
       </c>
       <c r="D81">
-        <v>4.41</v>
+        <v>3.09</v>
       </c>
       <c r="E81">
-        <v>2.04</v>
+        <v>1.85</v>
       </c>
       <c r="F81">
-        <v>9.51</v>
+        <v>5.17</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -3672,24 +3669,24 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>True bacteraemia (evaluated retrospectively) - Yes</t>
+          <t>Aztreonam</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -3698,13 +3695,13 @@
         </is>
       </c>
       <c r="D82">
-        <v>0.13</v>
+        <v>0.28</v>
       </c>
       <c r="E82">
-        <v>0.06</v>
+        <v>0.19</v>
       </c>
       <c r="F82">
-        <v>0.28</v>
+        <v>0.41</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -3713,24 +3710,24 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>vancomycin resistance</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>vancomycin-resistant Enterococci</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>True bacteraemia (evaluated retrospectively) - Possible</t>
+          <t>Aminoglycosides-Gentamicin</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3739,13 +3736,13 @@
         </is>
       </c>
       <c r="D83">
-        <v>6.13</v>
+        <v>0.48</v>
       </c>
       <c r="E83">
-        <v>1.82</v>
+        <v>0.33</v>
       </c>
       <c r="F83">
-        <v>20.67</v>
+        <v>0.7</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -3754,24 +3751,24 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>mixed or unspecified population</t>
+          <t>high risk</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>vancomycin resistance</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>vancomycin-resistant Enterococci</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Treatment modalities - Intensity of treatment (ITR-3 level 4, most intensive treatment)</t>
+          <t>Aminoglycosides-Tobramycin</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3779,9 +3776,18 @@
           <t>Other</t>
         </is>
       </c>
+      <c r="D84">
+        <v>0.48</v>
+      </c>
+      <c r="E84">
+        <v>0.32</v>
+      </c>
+      <c r="F84">
+        <v>0.73</v>
+      </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Pediatrics</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -3791,19 +3797,19 @@
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>multiple AMR profiles combined</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Treatment modalities - Intensity of treatment (ITR-3 level 4, most intensive treatment)</t>
+          <t>Sulfonamides-Sulfame-thoxazole</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -3812,17 +3818,17 @@
         </is>
       </c>
       <c r="D85">
-        <v>2.32</v>
+        <v>0.52</v>
       </c>
       <c r="E85">
-        <v>1.18</v>
+        <v>0.35</v>
       </c>
       <c r="F85">
-        <v>4.56</v>
+        <v>0.77</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Pediatrics</t>
+          <t>Adults</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -3832,19 +3838,20 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>multiple AMR profiles combined</t>
+          <t>3rd gen cephalosporin resistance</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>other/combination of multiple pathogens</t>
+          <t>C3G-resistant Enterobacterales</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Altered consciousness</t>
+          <t>Prior piperacillin-tazobactam_x000D_
+exposure</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -3853,39 +3860,39 @@
         </is>
       </c>
       <c r="D86">
-        <v>11.75</v>
+        <v>3.39</v>
       </c>
       <c r="E86">
-        <v>1.99</v>
+        <v>2.51</v>
       </c>
       <c r="F86">
-        <v>69.41</v>
+        <v>4.57</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Pediatrics</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>resistance against multiple Watch antibiotics</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Combined infection - Perianal infection</t>
+          <t>Prior antifungal exposure</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -3894,39 +3901,39 @@
         </is>
       </c>
       <c r="D87">
-        <v>5.63</v>
+        <v>3.92</v>
       </c>
       <c r="E87">
-        <v>1.99</v>
+        <v>1.35</v>
       </c>
       <c r="F87">
-        <v>15.94</v>
+        <v>11.37</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Adults</t>
+          <t>All ages or not specified</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>high risk</t>
+          <t>mixed or unspecified population</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>carbapenem resistance</t>
+          <t>resistance against multiple Watch antibiotics</t>
         </is>
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>carbapenem-resistant Enterobacterales</t>
+          <t>other/combination of multiple pathogens</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Combined infection - Perianal infection</t>
+          <t>Time between admission and index culture days - 1 day prior to admission</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -3934,6 +3941,15 @@
           <t>Other</t>
         </is>
       </c>
+      <c r="D88">
+        <v>1.05</v>
+      </c>
+      <c r="E88">
+        <v>0.68</v>
+      </c>
+      <c r="F88">
+        <v>1.63</v>
+      </c>
       <c r="G88" t="inlineStr">
         <is>
           <t>Adults</t>
@@ -3941,15 +3957,334 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
+          <t>mixed or unspecified population</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>carbapenem resistance</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>carbapenem-resistant Enterobacterales</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Time between admission and index culture days - Same day as admission</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D89">
+        <v>0.48</v>
+      </c>
+      <c r="E89">
+        <v>0.35</v>
+      </c>
+      <c r="F89">
+        <v>0.65</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Adults</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>mixed or unspecified population</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>carbapenem resistance</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>carbapenem-resistant Enterobacterales</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Type of infection - Bacteraemia</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D90">
+        <v>4.68</v>
+      </c>
+      <c r="E90">
+        <v>1.79</v>
+      </c>
+      <c r="F90">
+        <v>12.23</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Adults</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>mixed or unspecified population</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>MDR</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>other/combination of multiple pathogens</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Receipt of inotropic drug</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D91">
+        <v>4.41</v>
+      </c>
+      <c r="E91">
+        <v>2.04</v>
+      </c>
+      <c r="F91">
+        <v>9.51</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Adults</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>mixed or unspecified population</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>carbapenem resistance</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>carbapenem-resistant Enterobacterales</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>True bacteraemia (evaluated retrospectively) - Yes</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D92">
+        <v>0.13</v>
+      </c>
+      <c r="E92">
+        <v>0.06</v>
+      </c>
+      <c r="F92">
+        <v>0.28</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Adults</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>mixed or unspecified population</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>vancomycin resistance</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>vancomycin-resistant Enterococci</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>True bacteraemia (evaluated retrospectively) - Possible</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D93">
+        <v>6.13</v>
+      </c>
+      <c r="E93">
+        <v>1.82</v>
+      </c>
+      <c r="F93">
+        <v>20.67</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Adults</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>mixed or unspecified population</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>vancomycin resistance</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>vancomycin-resistant Enterococci</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Antimicrobial use before KP isolation - Antifungals</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D94">
+        <v>4.13</v>
+      </c>
+      <c r="E94">
+        <v>2.31</v>
+      </c>
+      <c r="F94">
+        <v>7.38</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Adults</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>mixed or unspecified population</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>carbapenem resistance</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>carbapenem-resistant Enterobacterales</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Treatment modalities - Intensity of treatment (ITR-3 level 4, most intensive treatment)</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Pediatrics</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
           <t>high risk</t>
         </is>
       </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>MDR</t>
-        </is>
-      </c>
-      <c r="J88" t="inlineStr">
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>multiple AMR profiles combined</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>other/combination of multiple pathogens</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Treatment modalities - Intensity of treatment (ITR-3 level 4, most intensive treatment)</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D96">
+        <v>2.32</v>
+      </c>
+      <c r="E96">
+        <v>1.18</v>
+      </c>
+      <c r="F96">
+        <v>4.56</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Pediatrics</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>high risk</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>multiple AMR profiles combined</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
         <is>
           <t>other/combination of multiple pathogens</t>
         </is>

</xml_diff>